<commit_message>
Final dohee's commit during working with team (#22)
* Modify incorrect sport facility file

* Update 2021 parental_leave

* Analysis of correlation

* summarization process

* Analysis of correlation

* final commit today

---------

Co-authored-by: bukdohee <dohee1733@gmail.com>
</commit_message>
<xml_diff>
--- a/data/dohee/0_데이터 전처리 전/영유아 자료/2008-2022_총 영유아(만 0-6세) 계산 과정.xlsx
+++ b/data/dohee/0_데이터 전처리 전/영유아 자료/2008-2022_총 영유아(만 0-6세) 계산 과정.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\playdata\ML_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\playdata\To_raise_a_child_well\data\dohee\0_데이터 전처리 전\영유아 자료\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEE77C1-CB0E-4092-9E49-025BDAA8BDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C0A75A-5D8B-4B1D-B236-1A65EB9C7254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5BDC6609-0C90-4D57-BAD3-05C007F2CF73}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="영유아수" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="50">
   <si>
     <t>행정기관</t>
   </si>
@@ -433,7 +434,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -486,6 +487,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -802,11 +806,969 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E874A98-A93C-4F1F-8431-8D8008702ED2}">
+  <dimension ref="A2:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="19.09765625" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.19921875" customWidth="1"/>
+    <col min="14" max="15" width="11.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="10" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3277632</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3229577</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3208694</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3212933</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3265160</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3264476</v>
+      </c>
+      <c r="H4" s="4">
+        <v>3210156</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3187718</v>
+      </c>
+      <c r="J4" s="4">
+        <v>3153489</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3044577</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2904953</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2726967</v>
+      </c>
+      <c r="N4" s="4">
+        <v>2562100</v>
+      </c>
+      <c r="O4" s="4">
+        <v>2387763</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>612207</v>
+      </c>
+      <c r="C5" s="4">
+        <v>600593</v>
+      </c>
+      <c r="D5" s="4">
+        <v>588203</v>
+      </c>
+      <c r="E5" s="4">
+        <v>579444</v>
+      </c>
+      <c r="F5" s="4">
+        <v>581694</v>
+      </c>
+      <c r="G5" s="4">
+        <v>574126</v>
+      </c>
+      <c r="H5" s="4">
+        <v>559662</v>
+      </c>
+      <c r="I5" s="4">
+        <v>546824</v>
+      </c>
+      <c r="J5" s="4">
+        <v>530484</v>
+      </c>
+      <c r="K5" s="4">
+        <v>504604</v>
+      </c>
+      <c r="L5" s="4">
+        <v>471155</v>
+      </c>
+      <c r="M5" s="4">
+        <v>438969</v>
+      </c>
+      <c r="N5" s="4">
+        <v>407374</v>
+      </c>
+      <c r="O5" s="4">
+        <v>375106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>186794</v>
+      </c>
+      <c r="C6" s="4">
+        <v>182462</v>
+      </c>
+      <c r="D6" s="4">
+        <v>180025</v>
+      </c>
+      <c r="E6" s="4">
+        <v>180967</v>
+      </c>
+      <c r="F6" s="4">
+        <v>185269</v>
+      </c>
+      <c r="G6" s="4">
+        <v>187305</v>
+      </c>
+      <c r="H6" s="4">
+        <v>186105</v>
+      </c>
+      <c r="I6" s="4">
+        <v>187693</v>
+      </c>
+      <c r="J6" s="4">
+        <v>187409</v>
+      </c>
+      <c r="K6" s="4">
+        <v>180213</v>
+      </c>
+      <c r="L6" s="4">
+        <v>171569</v>
+      </c>
+      <c r="M6" s="4">
+        <v>159957</v>
+      </c>
+      <c r="N6" s="4">
+        <v>150182</v>
+      </c>
+      <c r="O6" s="4">
+        <v>138947</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>151952</v>
+      </c>
+      <c r="C7" s="4">
+        <v>148663</v>
+      </c>
+      <c r="D7" s="4">
+        <v>145683</v>
+      </c>
+      <c r="E7" s="4">
+        <v>145045</v>
+      </c>
+      <c r="F7" s="4">
+        <v>146806</v>
+      </c>
+      <c r="G7" s="4">
+        <v>146696</v>
+      </c>
+      <c r="H7" s="4">
+        <v>143732</v>
+      </c>
+      <c r="I7" s="4">
+        <v>142823</v>
+      </c>
+      <c r="J7" s="4">
+        <v>142275</v>
+      </c>
+      <c r="K7" s="4">
+        <v>137711</v>
+      </c>
+      <c r="L7" s="4">
+        <v>131434</v>
+      </c>
+      <c r="M7" s="4">
+        <v>122898</v>
+      </c>
+      <c r="N7" s="4">
+        <v>114490</v>
+      </c>
+      <c r="O7" s="4">
+        <v>105524</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5">
+        <v>181653</v>
+      </c>
+      <c r="C8" s="4">
+        <v>179748</v>
+      </c>
+      <c r="D8" s="4">
+        <v>178318</v>
+      </c>
+      <c r="E8" s="4">
+        <v>183250</v>
+      </c>
+      <c r="F8" s="4">
+        <v>190111</v>
+      </c>
+      <c r="G8" s="4">
+        <v>192549</v>
+      </c>
+      <c r="H8" s="4">
+        <v>190178</v>
+      </c>
+      <c r="I8" s="4">
+        <v>189521</v>
+      </c>
+      <c r="J8" s="4">
+        <v>186583</v>
+      </c>
+      <c r="K8" s="4">
+        <v>178698</v>
+      </c>
+      <c r="L8" s="4">
+        <v>169605</v>
+      </c>
+      <c r="M8" s="4">
+        <v>158855</v>
+      </c>
+      <c r="N8" s="4">
+        <v>147412</v>
+      </c>
+      <c r="O8" s="4">
+        <v>138349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5">
+        <v>103614</v>
+      </c>
+      <c r="C9" s="4">
+        <v>102573</v>
+      </c>
+      <c r="D9" s="4">
+        <v>101468</v>
+      </c>
+      <c r="E9" s="4">
+        <v>101296</v>
+      </c>
+      <c r="F9" s="4">
+        <v>102549</v>
+      </c>
+      <c r="G9" s="4">
+        <v>102130</v>
+      </c>
+      <c r="H9" s="4">
+        <v>99665</v>
+      </c>
+      <c r="I9" s="4">
+        <v>97599</v>
+      </c>
+      <c r="J9" s="4">
+        <v>95232</v>
+      </c>
+      <c r="K9" s="4">
+        <v>91407</v>
+      </c>
+      <c r="L9" s="4">
+        <v>86978</v>
+      </c>
+      <c r="M9" s="4">
+        <v>81232</v>
+      </c>
+      <c r="N9" s="4">
+        <v>75795</v>
+      </c>
+      <c r="O9" s="4">
+        <v>71441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>106136</v>
+      </c>
+      <c r="C10" s="4">
+        <v>103942</v>
+      </c>
+      <c r="D10" s="4">
+        <v>102962</v>
+      </c>
+      <c r="E10" s="4">
+        <v>103693</v>
+      </c>
+      <c r="F10" s="4">
+        <v>105569</v>
+      </c>
+      <c r="G10" s="4">
+        <v>106057</v>
+      </c>
+      <c r="H10" s="4">
+        <v>103199</v>
+      </c>
+      <c r="I10" s="4">
+        <v>99724</v>
+      </c>
+      <c r="J10" s="4">
+        <v>97680</v>
+      </c>
+      <c r="K10" s="4">
+        <v>92647</v>
+      </c>
+      <c r="L10" s="4">
+        <v>86476</v>
+      </c>
+      <c r="M10" s="4">
+        <v>79447</v>
+      </c>
+      <c r="N10" s="4">
+        <v>73389</v>
+      </c>
+      <c r="O10" s="4">
+        <v>68117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5">
+        <v>78808</v>
+      </c>
+      <c r="C11" s="4">
+        <v>77758</v>
+      </c>
+      <c r="D11" s="4">
+        <v>77069</v>
+      </c>
+      <c r="E11" s="4">
+        <v>78133</v>
+      </c>
+      <c r="F11" s="4">
+        <v>80473</v>
+      </c>
+      <c r="G11" s="4">
+        <v>81651</v>
+      </c>
+      <c r="H11" s="4">
+        <v>81650</v>
+      </c>
+      <c r="I11" s="4">
+        <v>81922</v>
+      </c>
+      <c r="J11" s="4">
+        <v>81221</v>
+      </c>
+      <c r="K11" s="4">
+        <v>78312</v>
+      </c>
+      <c r="L11" s="4">
+        <v>74028</v>
+      </c>
+      <c r="M11" s="4">
+        <v>68923</v>
+      </c>
+      <c r="N11" s="4">
+        <v>63769</v>
+      </c>
+      <c r="O11" s="4">
+        <v>57970</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4">
+        <v>8542</v>
+      </c>
+      <c r="G12" s="4">
+        <v>9499</v>
+      </c>
+      <c r="H12" s="4">
+        <v>13934</v>
+      </c>
+      <c r="I12" s="4">
+        <v>20941</v>
+      </c>
+      <c r="J12" s="4">
+        <v>24353</v>
+      </c>
+      <c r="K12" s="4">
+        <v>27793</v>
+      </c>
+      <c r="L12" s="4">
+        <v>30508</v>
+      </c>
+      <c r="M12" s="4">
+        <v>31742</v>
+      </c>
+      <c r="N12" s="4">
+        <v>31317</v>
+      </c>
+      <c r="O12" s="4">
+        <v>30746</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
+        <v>862079</v>
+      </c>
+      <c r="C13" s="4">
+        <v>855744</v>
+      </c>
+      <c r="D13" s="4">
+        <v>862009</v>
+      </c>
+      <c r="E13" s="4">
+        <v>865227</v>
+      </c>
+      <c r="F13" s="4">
+        <v>881034</v>
+      </c>
+      <c r="G13" s="4">
+        <v>881883</v>
+      </c>
+      <c r="H13" s="4">
+        <v>866844</v>
+      </c>
+      <c r="I13" s="4">
+        <v>862159</v>
+      </c>
+      <c r="J13" s="4">
+        <v>860224</v>
+      </c>
+      <c r="K13" s="4">
+        <v>838610</v>
+      </c>
+      <c r="L13" s="4">
+        <v>816247</v>
+      </c>
+      <c r="M13" s="4">
+        <v>776603</v>
+      </c>
+      <c r="N13" s="4">
+        <v>743268</v>
+      </c>
+      <c r="O13" s="4">
+        <v>702824</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5">
+        <v>93516</v>
+      </c>
+      <c r="C14" s="4">
+        <v>91288</v>
+      </c>
+      <c r="D14" s="4">
+        <v>89715</v>
+      </c>
+      <c r="E14" s="4">
+        <v>88462</v>
+      </c>
+      <c r="F14" s="4">
+        <v>88422</v>
+      </c>
+      <c r="G14" s="4">
+        <v>87391</v>
+      </c>
+      <c r="H14" s="4">
+        <v>84976</v>
+      </c>
+      <c r="I14" s="4">
+        <v>83855</v>
+      </c>
+      <c r="J14" s="4">
+        <v>81964</v>
+      </c>
+      <c r="K14" s="4">
+        <v>78458</v>
+      </c>
+      <c r="L14" s="4">
+        <v>74334</v>
+      </c>
+      <c r="M14" s="4">
+        <v>70577</v>
+      </c>
+      <c r="N14" s="4">
+        <v>67866</v>
+      </c>
+      <c r="O14" s="4">
+        <v>64676</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5">
+        <v>101382</v>
+      </c>
+      <c r="C15" s="4">
+        <v>100023</v>
+      </c>
+      <c r="D15" s="4">
+        <v>100252</v>
+      </c>
+      <c r="E15" s="4">
+        <v>100985</v>
+      </c>
+      <c r="F15" s="4">
+        <v>102070</v>
+      </c>
+      <c r="G15" s="4">
+        <v>102064</v>
+      </c>
+      <c r="H15" s="4">
+        <v>99865</v>
+      </c>
+      <c r="I15" s="4">
+        <v>98631</v>
+      </c>
+      <c r="J15" s="4">
+        <v>97656</v>
+      </c>
+      <c r="K15" s="4">
+        <v>94031</v>
+      </c>
+      <c r="L15" s="4">
+        <v>90073</v>
+      </c>
+      <c r="M15" s="4">
+        <v>84531</v>
+      </c>
+      <c r="N15" s="4">
+        <v>79742</v>
+      </c>
+      <c r="O15" s="4">
+        <v>74651</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5">
+        <v>137723</v>
+      </c>
+      <c r="C16" s="4">
+        <v>138021</v>
+      </c>
+      <c r="D16" s="4">
+        <v>139744</v>
+      </c>
+      <c r="E16" s="4">
+        <v>142123</v>
+      </c>
+      <c r="F16" s="4">
+        <v>139185</v>
+      </c>
+      <c r="G16" s="4">
+        <v>139918</v>
+      </c>
+      <c r="H16" s="4">
+        <v>137570</v>
+      </c>
+      <c r="I16" s="4">
+        <v>136809</v>
+      </c>
+      <c r="J16" s="4">
+        <v>136336</v>
+      </c>
+      <c r="K16" s="4">
+        <v>133264</v>
+      </c>
+      <c r="L16" s="4">
+        <v>127566</v>
+      </c>
+      <c r="M16" s="4">
+        <v>118988</v>
+      </c>
+      <c r="N16" s="4">
+        <v>111235</v>
+      </c>
+      <c r="O16" s="4">
+        <v>103232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5">
+        <v>117602</v>
+      </c>
+      <c r="C17" s="4">
+        <v>114887</v>
+      </c>
+      <c r="D17" s="4">
+        <v>113481</v>
+      </c>
+      <c r="E17" s="4">
+        <v>113344</v>
+      </c>
+      <c r="F17" s="4">
+        <v>114150</v>
+      </c>
+      <c r="G17" s="4">
+        <v>113709</v>
+      </c>
+      <c r="H17" s="4">
+        <v>110999</v>
+      </c>
+      <c r="I17" s="4">
+        <v>108996</v>
+      </c>
+      <c r="J17" s="4">
+        <v>106734</v>
+      </c>
+      <c r="K17" s="4">
+        <v>101312</v>
+      </c>
+      <c r="L17" s="4">
+        <v>94615</v>
+      </c>
+      <c r="M17" s="4">
+        <v>86986</v>
+      </c>
+      <c r="N17" s="4">
+        <v>80434</v>
+      </c>
+      <c r="O17" s="4">
+        <v>73604</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5">
+        <v>116649</v>
+      </c>
+      <c r="C18" s="4">
+        <v>113212</v>
+      </c>
+      <c r="D18" s="4">
+        <v>111547</v>
+      </c>
+      <c r="E18" s="4">
+        <v>111225</v>
+      </c>
+      <c r="F18" s="4">
+        <v>112748</v>
+      </c>
+      <c r="G18" s="4">
+        <v>112187</v>
+      </c>
+      <c r="H18" s="4">
+        <v>109834</v>
+      </c>
+      <c r="I18" s="4">
+        <v>109694</v>
+      </c>
+      <c r="J18" s="4">
+        <v>108200</v>
+      </c>
+      <c r="K18" s="4">
+        <v>103413</v>
+      </c>
+      <c r="L18" s="4">
+        <v>97018</v>
+      </c>
+      <c r="M18" s="4">
+        <v>90196</v>
+      </c>
+      <c r="N18" s="4">
+        <v>84424</v>
+      </c>
+      <c r="O18" s="4">
+        <v>77930</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5">
+        <v>162967</v>
+      </c>
+      <c r="C19" s="4">
+        <v>158597</v>
+      </c>
+      <c r="D19" s="4">
+        <v>157003</v>
+      </c>
+      <c r="E19" s="4">
+        <v>157738</v>
+      </c>
+      <c r="F19" s="4">
+        <v>159769</v>
+      </c>
+      <c r="G19" s="4">
+        <v>159692</v>
+      </c>
+      <c r="H19" s="4">
+        <v>157132</v>
+      </c>
+      <c r="I19" s="4">
+        <v>156764</v>
+      </c>
+      <c r="J19" s="4">
+        <v>155467</v>
+      </c>
+      <c r="K19" s="4">
+        <v>149782</v>
+      </c>
+      <c r="L19" s="4">
+        <v>141547</v>
+      </c>
+      <c r="M19" s="4">
+        <v>131841</v>
+      </c>
+      <c r="N19" s="4">
+        <v>122242</v>
+      </c>
+      <c r="O19" s="4">
+        <v>113044</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="5">
+        <v>222172</v>
+      </c>
+      <c r="C20" s="4">
+        <v>220807</v>
+      </c>
+      <c r="D20" s="4">
+        <v>220576</v>
+      </c>
+      <c r="E20" s="4">
+        <v>221388</v>
+      </c>
+      <c r="F20" s="4">
+        <v>225299</v>
+      </c>
+      <c r="G20" s="4">
+        <v>225581</v>
+      </c>
+      <c r="H20" s="4">
+        <v>222564</v>
+      </c>
+      <c r="I20" s="4">
+        <v>220697</v>
+      </c>
+      <c r="J20" s="4">
+        <v>217810</v>
+      </c>
+      <c r="K20" s="4">
+        <v>210705</v>
+      </c>
+      <c r="L20" s="4">
+        <v>199210</v>
+      </c>
+      <c r="M20" s="4">
+        <v>184918</v>
+      </c>
+      <c r="N20" s="4">
+        <v>170795</v>
+      </c>
+      <c r="O20" s="4">
+        <v>155419</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5">
+        <v>42378</v>
+      </c>
+      <c r="C21" s="4">
+        <v>41259</v>
+      </c>
+      <c r="D21" s="4">
+        <v>40639</v>
+      </c>
+      <c r="E21" s="4">
+        <v>40613</v>
+      </c>
+      <c r="F21" s="4">
+        <v>41470</v>
+      </c>
+      <c r="G21" s="4">
+        <v>42038</v>
+      </c>
+      <c r="H21" s="4">
+        <v>42247</v>
+      </c>
+      <c r="I21" s="4">
+        <v>43066</v>
+      </c>
+      <c r="J21" s="4">
+        <v>43861</v>
+      </c>
+      <c r="K21" s="4">
+        <v>43617</v>
+      </c>
+      <c r="L21" s="4">
+        <v>42590</v>
+      </c>
+      <c r="M21" s="4">
+        <v>40304</v>
+      </c>
+      <c r="N21" s="4">
+        <v>38366</v>
+      </c>
+      <c r="O21" s="4">
+        <v>36183</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000CE42E-4A1D-4BEF-A782-D9C17AE56157}">
   <dimension ref="A2:AQ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T1" activeCellId="6" sqref="B1:D1048576 E1:G1048576 H1:J1048576 K1:M1048576 N1:P1048576 Q1:S1048576 T1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -855,76 +1817,76 @@
   <sheetData>
     <row r="2" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12" t="s">
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12" t="s">
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12" t="s">
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12" t="s">
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12" t="s">
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12" t="s">
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12" t="s">
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="12" t="s">
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12" t="s">
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AM2" s="12"/>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12" t="s">
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="18"/>
     </row>
     <row r="3" spans="1:43" s="10" customFormat="1" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
@@ -3665,12 +4627,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
     <mergeCell ref="AL2:AN2"/>
     <mergeCell ref="AO2:AQ2"/>
     <mergeCell ref="T2:V2"/>
@@ -3679,13 +4635,19 @@
     <mergeCell ref="AC2:AE2"/>
     <mergeCell ref="AF2:AH2"/>
     <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF94E224-2517-49E0-A84B-CCE3C64CE9D9}">
   <dimension ref="A3:T29"/>
   <sheetViews>

</xml_diff>